<commit_message>
final version, everything ready
</commit_message>
<xml_diff>
--- a/MUH PRE/ArbeitsProtokollSmartGastro.xlsx
+++ b/MUH PRE/ArbeitsProtokollSmartGastro.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elias\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PUBLIC\5AHIF\SYP_SmartGastro\MUH PRE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE759057-B1B6-47C1-B764-A4A311DFE3FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9B20C0-52DC-4942-BE84-227B91E42360}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AE33E597-1370-421D-8CDB-6615D11E929F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
   <si>
     <t>Lotteritsch</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Erstellung von Testdaten in der Datenbank für das Webserivce</t>
   </si>
   <si>
-    <t>Fertigstellung des HTTP-Serivce im Frontend um Daten vom Webservice zu bekommen</t>
-  </si>
-  <si>
     <t>Weitere Aufbereitung der Testdaten, sowie überlegung von anderen Implementierung der Datenbank</t>
   </si>
   <si>
@@ -146,17 +143,83 @@
     <t>Fixing Bugs in der WebApp</t>
   </si>
   <si>
-    <t>Arbeiten an der Android App, erstellung des Bestellmenüs in der Android App</t>
-  </si>
-  <si>
     <t xml:space="preserve">Weiterarbeiten am Webservice </t>
+  </si>
+  <si>
+    <t>Fertigstellung des HTTP-Service im Frontend um Daten vom Webservice zu bekommen</t>
+  </si>
+  <si>
+    <t>Arbeiten an der Android App, Erstellung des Bestellmenüs in der Android App</t>
+  </si>
+  <si>
+    <t>Weiterarbeiten an der Weboberfläche</t>
+  </si>
+  <si>
+    <t>Besprechung für nächste Iteration</t>
+  </si>
+  <si>
+    <t>Weitere Pläne Iteration 3</t>
+  </si>
+  <si>
+    <t>Stunden</t>
+  </si>
+  <si>
+    <t>Routen für Warenkorb</t>
+  </si>
+  <si>
+    <t>Gebrachte Produkte abhaken</t>
+  </si>
+  <si>
+    <t>Warenkorb der Android App</t>
+  </si>
+  <si>
+    <t>Helfen bei Melisa bei App</t>
+  </si>
+  <si>
+    <t>Warenkorb der Android App / schickt nicht richtig ab</t>
+  </si>
+  <si>
+    <t>Meeting Teams</t>
+  </si>
+  <si>
+    <t>Firebase kennenlernen, Firestore erstellen, verstehen, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Feedback App mit Android</t>
+  </si>
+  <si>
+    <t>Besprechung derzeitiger Stand</t>
+  </si>
+  <si>
+    <t>Datenbankänderungen</t>
+  </si>
+  <si>
+    <t>Bugs Androidapp</t>
+  </si>
+  <si>
+    <t>Design und paar Kleinigkeiten, schöner machen</t>
+  </si>
+  <si>
+    <t>gesamt</t>
+  </si>
+  <si>
+    <t>E. Mikula</t>
+  </si>
+  <si>
+    <t>A. Lotteritsch</t>
+  </si>
+  <si>
+    <t>M. Dizdarevic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +250,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -206,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -282,6 +359,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -289,11 +403,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -313,6 +424,42 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -634,250 +781,716 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0AD46E-7585-403C-980D-02C49E242217}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.77734375" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>43738</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="E4" s="22">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>43745</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="E5" s="22">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>43752</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="E6" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>43759</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="E7" s="22">
+        <v>2</v>
+      </c>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>43766</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="E8" s="22">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>43773</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="E9" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>43780</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="E10" s="22">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>43787</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>43794</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>43794</v>
-      </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>43801</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>43801</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="E13" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>43808</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>43815</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>43843</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>43808</v>
-      </c>
-      <c r="B14" s="8" t="s">
+      <c r="E16" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>43850</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>43852</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>43815</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="E18" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>43853</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>43857</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>43859</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>43860</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>43864</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>43866</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>43871</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <v>43843</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>43850</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="D25" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>43873</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D26" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>43878</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>35</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>43880</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>43885</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>43887</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>43888</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>43892</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>43894</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>43899</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>43901</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>43902</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>43928</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="17">
+        <v>43931</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="18"/>
+      <c r="D38" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="17">
+        <v>43937</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="17">
+        <v>43938</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D41" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="23">
+        <f>SUM(E4:E40)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D42" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="23">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D43" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="23">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D44" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" s="23">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D2"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>